<commit_message>
fixed player bullet direction
</commit_message>
<xml_diff>
--- a/enemy_bullets.xlsx
+++ b/enemy_bullets.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
   <si>
     <t>SourceType</t>
   </si>
@@ -93,16 +93,16 @@
     <t>BulletTypes</t>
   </si>
   <si>
-    <t>LocalX</t>
+    <t>SpawnX</t>
   </si>
   <si>
-    <t>LocalY</t>
+    <t>SpawnY</t>
   </si>
   <si>
-    <t>LocalXQ7</t>
+    <t>SpawnXQ7</t>
   </si>
   <si>
-    <t>LocalYQ7</t>
+    <t>SpawnYQ7</t>
   </si>
   <si>
     <t>ValidateLocalXY</t>
@@ -126,10 +126,16 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>LocalXQ7</t>
+  </si>
+  <si>
     <t>int8_t</t>
   </si>
   <si>
     <t>Bullet_Enemy_Normal_1</t>
+  </si>
+  <si>
+    <t>LocalYQ7</t>
   </si>
   <si>
     <t>Bullet_Enemy_Normal_5</t>
@@ -382,10 +388,10 @@
     <tableColumn name="Quantity" id="4"/>
     <tableColumn name="TimeDelay" id="5"/>
     <tableColumn name="BulletTypes" id="6"/>
-    <tableColumn name="LocalX" id="7"/>
-    <tableColumn name="LocalY" id="8"/>
-    <tableColumn name="LocalXQ7" id="9"/>
-    <tableColumn name="LocalYQ7" id="10"/>
+    <tableColumn name="SpawnX" id="7"/>
+    <tableColumn name="SpawnY" id="8"/>
+    <tableColumn name="SpawnXQ7" id="9"/>
+    <tableColumn name="SpawnYQ7" id="10"/>
     <tableColumn name="ValidateLocalXY" id="11"/>
     <tableColumn name="SourceIndex" id="12"/>
     <tableColumn name="TimeCastQ4" id="13"/>
@@ -5750,8 +5756,8 @@
     <col customWidth="1" min="5" max="5" width="9.13"/>
     <col customWidth="1" min="6" max="6" width="20.13"/>
     <col customWidth="1" min="7" max="8" width="12.88"/>
-    <col customWidth="1" min="9" max="9" width="8.75"/>
-    <col customWidth="1" min="10" max="10" width="9.0"/>
+    <col customWidth="1" min="9" max="9" width="9.75"/>
+    <col customWidth="1" min="10" max="10" width="9.63"/>
     <col customWidth="1" min="11" max="11" width="13.63"/>
     <col customWidth="1" min="12" max="12" width="11.38"/>
     <col customWidth="1" min="13" max="13" width="10.88"/>
@@ -5889,10 +5895,10 @@
         <v>1</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
@@ -5912,7 +5918,7 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G3" s="8">
         <v>0.0</v>
@@ -5958,10 +5964,10 @@
         <v>1</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
@@ -5981,7 +5987,7 @@
         <v>0.0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8">
         <v>0.0</v>
@@ -6050,7 +6056,7 @@
         <v>0.15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G5" s="8">
         <v>0.0</v>
@@ -6119,7 +6125,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G6" s="8">
         <v>-0.5</v>
@@ -6188,7 +6194,7 @@
         <v>0.0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G7" s="8">
         <v>-0.07279745795169545</v>
@@ -6232,10 +6238,10 @@
         <v>20</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="V7" s="4"/>
       <c r="W7" s="10" t="b">
@@ -6266,7 +6272,7 @@
         <v>0.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G8" s="8">
         <v>-0.8335103290849545</v>
@@ -6335,7 +6341,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G9" s="8">
         <v>0.0</v>
@@ -6398,7 +6404,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G10" s="8">
         <v>-0.1</v>
@@ -6461,13 +6467,13 @@
         <v>0.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G11" s="8">
         <v>0.1</v>
       </c>
-      <c r="H11" s="8">
-        <v>0.1</v>
+      <c r="H11" s="1">
+        <v>-0.1</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" ref="I11:J11" si="22">INT(G11 * 128)</f>
@@ -6475,7 +6481,7 @@
       </c>
       <c r="J11" s="9">
         <f t="shared" si="22"/>
-        <v>12</v>
+        <v>-13</v>
       </c>
       <c r="K11" s="9" t="b">
         <f t="shared" si="4"/>
@@ -6524,7 +6530,7 @@
         <v>0.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G12" s="8">
         <v>0.0</v>
@@ -25365,16 +25371,16 @@
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="5" t="s">
@@ -25407,7 +25413,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1">
         <v>0.25</v>
@@ -25429,7 +25435,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
@@ -25477,7 +25483,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>8</v>
@@ -25503,7 +25509,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1">
         <v>0.09</v>
@@ -25545,7 +25551,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1">
         <v>0.15</v>
@@ -25587,7 +25593,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>0.05</v>
@@ -25629,7 +25635,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1">
         <v>0.3</v>

</xml_diff>